<commit_message>
[external commands] - [`tail(id,file)`]: simulate the *NIX tail command.
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/showcase/artifact/data/external-showcase.data.xlsx
+++ b/src/test/resources/showcase/artifact/data/external-showcase.data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/src/test/resources/showcase/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2190151E-EF6C-5F4A-9E99-12CBDEDF02BE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{573DC404-F691-9745-8E43-D2648396F79B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="10500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="-21140" windowWidth="11760" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -574,7 +574,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>

</xml_diff>